<commit_message>
update 1018 12 PM
</commit_message>
<xml_diff>
--- a/Data/GGEE_23_School Districts_table.xlsx
+++ b/Data/GGEE_23_School Districts_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristachisholm/Documents/GitHub/GGEESummer23/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B6FBFE-AA85-A140-9EA3-65B712493533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A9229D1-C0E1-E14C-A8EA-8D4AEE624FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1760" yWindow="740" windowWidth="27640" windowHeight="16920" activeTab="1" xr2:uid="{9D128637-DA45-8E47-9429-C54E0C6FC649}"/>
   </bookViews>
@@ -141,25 +141,25 @@
     <t>Introductory</t>
   </si>
   <si>
-    <t>Local Funding</t>
-  </si>
-  <si>
     <t>UF Donor Funding</t>
   </si>
   <si>
-    <t>City Funded</t>
-  </si>
-  <si>
-    <t>UF - GGEE Donor Funding</t>
-  </si>
-  <si>
-    <t>District Funding</t>
-  </si>
-  <si>
-    <t>Program Funding</t>
-  </si>
-  <si>
     <t>Number of Programs</t>
+  </si>
+  <si>
+    <t>Program Funding Sources</t>
+  </si>
+  <si>
+    <t>City Funded, State AI, GGEE</t>
+  </si>
+  <si>
+    <t>GGEE Donor Funding, , State AI</t>
+  </si>
+  <si>
+    <t>District Funding, State AI, GGEE</t>
+  </si>
+  <si>
+    <t>Local Funding, State AI, GGEE</t>
   </si>
 </sst>
 </file>
@@ -314,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -326,8 +326,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -615,7 +613,7 @@
   </sortState>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{59B91786-BEB3-0F45-91F0-893A45B7971B}" name="School District" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{A55BF806-DF69-0641-8725-E1A95CC28175}" name="Program Funding" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{A55BF806-DF69-0641-8725-E1A95CC28175}" name="Program Funding Sources" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{B19C62A5-B091-FD42-9660-32E83F25C71B}" name="Number of Programs" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1268,13 +1266,13 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="36.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1283,10 +1281,10 @@
         <v>14</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>40</v>
+        <v>36</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1294,9 +1292,9 @@
         <v>17</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="11">
+        <v>40</v>
+      </c>
+      <c r="C2">
         <v>1</v>
       </c>
     </row>
@@ -1305,9 +1303,9 @@
         <v>26</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="11">
+        <v>34</v>
+      </c>
+      <c r="C3">
         <v>1</v>
       </c>
     </row>
@@ -1316,9 +1314,9 @@
         <v>21</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="11">
+        <v>37</v>
+      </c>
+      <c r="C4">
         <v>1</v>
       </c>
     </row>
@@ -1327,9 +1325,9 @@
         <v>18</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="11">
+        <v>38</v>
+      </c>
+      <c r="C5">
         <v>2</v>
       </c>
     </row>
@@ -1338,9 +1336,9 @@
         <v>19</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="11">
+        <v>39</v>
+      </c>
+      <c r="C6">
         <v>4</v>
       </c>
     </row>
@@ -1349,9 +1347,9 @@
         <v>23</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="11">
+        <v>39</v>
+      </c>
+      <c r="C7">
         <v>2</v>
       </c>
     </row>
@@ -1360,9 +1358,9 @@
         <v>24</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="11">
+        <v>39</v>
+      </c>
+      <c r="C8">
         <v>6</v>
       </c>
     </row>
@@ -1371,9 +1369,9 @@
         <v>25</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="11">
+        <v>39</v>
+      </c>
+      <c r="C9">
         <v>2</v>
       </c>
     </row>
@@ -1382,9 +1380,9 @@
         <v>20</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="11">
+        <v>39</v>
+      </c>
+      <c r="C10">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update 1019 9 AM
</commit_message>
<xml_diff>
--- a/Data/GGEE_23_School Districts_table.xlsx
+++ b/Data/GGEE_23_School Districts_table.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristachisholm/Documents/GitHub/GGEESummer23/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristadulany/Documents/GitHub/GGEESummer23/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A9229D1-C0E1-E14C-A8EA-8D4AEE624FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069A504E-0D51-BC41-A8CF-CDFD292343E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1760" yWindow="740" windowWidth="27640" windowHeight="16920" activeTab="1" xr2:uid="{9D128637-DA45-8E47-9429-C54E0C6FC649}"/>
+    <workbookView xWindow="1760" yWindow="740" windowWidth="20420" windowHeight="13420" activeTab="1" xr2:uid="{9D128637-DA45-8E47-9429-C54E0C6FC649}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Support" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="43">
   <si>
     <t>Homestead Senior High School</t>
   </si>
@@ -150,22 +150,33 @@
     <t>Program Funding Sources</t>
   </si>
   <si>
-    <t>City Funded, State AI, GGEE</t>
-  </si>
-  <si>
-    <t>GGEE Donor Funding, , State AI</t>
-  </si>
-  <si>
-    <t>District Funding, State AI, GGEE</t>
-  </si>
-  <si>
-    <t>Local Funding, State AI, GGEE</t>
+    <t>State AI/GGEE Estimate</t>
+  </si>
+  <si>
+    <t>District/City Estimate</t>
+  </si>
+  <si>
+    <t>GGEE, State AI</t>
+  </si>
+  <si>
+    <t>City, State AI, GGEE</t>
+  </si>
+  <si>
+    <t>Local, State AI, GGEE</t>
+  </si>
+  <si>
+    <t>District, State AI, GGEE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="3">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -314,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -326,11 +337,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="17">
+    <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -590,31 +621,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CEC57D88-9219-5646-B2E7-C0516BAA3655}" name="Table1" displayName="Table1" ref="A1:D23" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13" totalsRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CEC57D88-9219-5646-B2E7-C0516BAA3655}" name="Table1" displayName="Table1" ref="A1:D23" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" totalsRowBorderDxfId="13">
   <autoFilter ref="A1:D23" xr:uid="{CEC57D88-9219-5646-B2E7-C0516BAA3655}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D23">
     <sortCondition ref="A1:A23"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{A2DD9F0B-E4AB-784B-B950-FFD4C0322493}" name="School District" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{A2369BB3-B453-7345-A95A-91E775585D2A}" name="School/Organization Name" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{CBE41D2B-943F-774B-8F37-AC9C9AECFA18}" name="Program Level" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{588F021C-66B5-0247-BAE5-4FD4C7344FA8}" name="Format" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{A2DD9F0B-E4AB-784B-B950-FFD4C0322493}" name="School District" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{A2369BB3-B453-7345-A95A-91E775585D2A}" name="School/Organization Name" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{CBE41D2B-943F-774B-8F37-AC9C9AECFA18}" name="Program Level" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{588F021C-66B5-0247-BAE5-4FD4C7344FA8}" name="Format" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0C877C3E-052E-4E49-9488-0BC6C14F1BD2}" name="Table13" displayName="Table13" ref="A1:C10" totalsRowShown="0" headerRowDxfId="6" dataDxfId="4" headerRowBorderDxfId="5" totalsRowBorderDxfId="3">
-  <autoFilter ref="A1:C10" xr:uid="{0C877C3E-052E-4E49-9488-0BC6C14F1BD2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0C877C3E-052E-4E49-9488-0BC6C14F1BD2}" name="Table13" displayName="Table13" ref="A1:E10" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" totalsRowBorderDxfId="5">
+  <autoFilter ref="A1:E10" xr:uid="{0C877C3E-052E-4E49-9488-0BC6C14F1BD2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B10">
     <sortCondition ref="A1:A10"/>
   </sortState>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{59B91786-BEB3-0F45-91F0-893A45B7971B}" name="School District" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{A55BF806-DF69-0641-8725-E1A95CC28175}" name="Program Funding Sources" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{B19C62A5-B091-FD42-9660-32E83F25C71B}" name="Number of Programs" dataDxfId="0"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{59B91786-BEB3-0F45-91F0-893A45B7971B}" name="School District" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{A55BF806-DF69-0641-8725-E1A95CC28175}" name="Program Funding Sources" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{B19C62A5-B091-FD42-9660-32E83F25C71B}" name="Number of Programs" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{A1C93DF7-0A7A-2B4F-A49E-C91D86442ADE}" name="State AI/GGEE Estimate" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{5B22C818-0D8E-B74E-8A45-5E29AF8C60EA}" name="District/City Estimate" dataDxfId="0">
+      <calculatedColumnFormula>SUM(#REF!,#REF!)</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1263,20 +1298,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD3E89B7-1488-E944-A807-6F1FDAF60FD9}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="36.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -1286,19 +1323,31 @@
       <c r="C1" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" s="11">
+        <v>450</v>
+      </c>
+      <c r="E2" s="12">
+        <v>4615</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
@@ -1308,83 +1357,134 @@
       <c r="C3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" s="11">
+        <v>4300</v>
+      </c>
+      <c r="E3" s="12">
+        <v>5900</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" s="11">
+        <v>2100</v>
+      </c>
+      <c r="E4" s="12">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" s="13">
+        <v>10342</v>
+      </c>
+      <c r="E5" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" s="11">
+        <v>6700</v>
+      </c>
+      <c r="E6" s="12">
+        <v>12700</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" s="11">
+        <v>3700</v>
+      </c>
+      <c r="E7" s="12">
+        <v>8100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C8">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" s="11">
+        <v>23000</v>
+      </c>
+      <c r="E8" s="12">
+        <v>18400</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" s="11">
+        <v>2000</v>
+      </c>
+      <c r="E9" s="12">
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C10">
         <v>3</v>
       </c>
+      <c r="D10" s="11">
+        <v>3300</v>
+      </c>
+      <c r="E10" s="12">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Final 1020 7 PM
</commit_message>
<xml_diff>
--- a/Data/GGEE_23_School Districts_table.xlsx
+++ b/Data/GGEE_23_School Districts_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristachisholm/Documents/GitHub/GGEESummer23/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6718C1BD-6F23-6E47-A763-731991CFF89D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A983D47C-DAA7-5940-BB1A-4C0B86F3C080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1760" yWindow="740" windowWidth="20420" windowHeight="13420" activeTab="1" xr2:uid="{9D128637-DA45-8E47-9429-C54E0C6FC649}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="63">
   <si>
     <t>Homestead Senior High School</t>
   </si>
@@ -177,30 +177,9 @@
     <t>$450</t>
   </si>
   <si>
-    <t>$4300</t>
-  </si>
-  <si>
-    <t>$2100</t>
-  </si>
-  <si>
-    <t>$10342</t>
-  </si>
-  <si>
-    <t>$6700</t>
-  </si>
-  <si>
-    <t>$3700</t>
-  </si>
-  <si>
-    <t>$23000</t>
-  </si>
-  <si>
     <t>$2000</t>
   </si>
   <si>
-    <t>$3300</t>
-  </si>
-  <si>
     <t>$4615</t>
   </si>
   <si>
@@ -222,15 +201,38 @@
     <t>$4600</t>
   </si>
   <si>
-    <t>$100</t>
+    <t>$4100</t>
+  </si>
+  <si>
+    <t>$29500</t>
+  </si>
+  <si>
+    <t>$27300</t>
+  </si>
+  <si>
+    <t>$11900</t>
+  </si>
+  <si>
+    <t>$71600</t>
+  </si>
+  <si>
+    <t>$15400</t>
+  </si>
+  <si>
+    <t>$38700</t>
+  </si>
+  <si>
+    <t>$500</t>
+  </si>
+  <si>
+    <t>$6300</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
@@ -382,7 +384,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
@@ -395,9 +397,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,6 +414,7 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -476,19 +478,19 @@
       </border>
     </dxf>
     <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -695,7 +697,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0C877C3E-052E-4E49-9488-0BC6C14F1BD2}" name="Table13" displayName="Table13" ref="A1:E10" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" totalsRowBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0C877C3E-052E-4E49-9488-0BC6C14F1BD2}" name="Table13" displayName="Table13" ref="A1:E10" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" headerRowBorderDxfId="6" totalsRowBorderDxfId="5">
   <autoFilter ref="A1:E10" xr:uid="{0C877C3E-052E-4E49-9488-0BC6C14F1BD2}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B10">
     <sortCondition ref="A1:A10"/>
@@ -705,9 +707,7 @@
     <tableColumn id="2" xr3:uid="{A55BF806-DF69-0641-8725-E1A95CC28175}" name="Funding Sources" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{B19C62A5-B091-FD42-9660-32E83F25C71B}" name="# Programs" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{A1C93DF7-0A7A-2B4F-A49E-C91D86442ADE}" name="UF Est" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{5B22C818-0D8E-B74E-8A45-5E29AF8C60EA}" name="Partner Est" dataDxfId="0">
-      <calculatedColumnFormula>SUM(#REF!,#REF!)</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="5" xr3:uid="{5B22C818-0D8E-B74E-8A45-5E29AF8C60EA}" name="Partner Est" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1356,22 +1356,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD3E89B7-1488-E944-A807-6F1FDAF60FD9}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
@@ -1401,11 +1401,12 @@
       <c r="D2" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E2" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="13"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
@@ -1416,13 +1417,14 @@
         <v>1</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="13"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>41</v>
       </c>
@@ -1433,13 +1435,14 @@
         <v>1</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="13"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -1449,14 +1452,15 @@
       <c r="C5">
         <v>2</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="14" t="s">
+      <c r="D5" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G5" s="13"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>19</v>
       </c>
@@ -1467,13 +1471,14 @@
         <v>4</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="13"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>23</v>
       </c>
@@ -1484,13 +1489,14 @@
         <v>2</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" s="13"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>24</v>
       </c>
@@ -1501,13 +1507,14 @@
         <v>6</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="13"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>25</v>
       </c>
@@ -1518,13 +1525,14 @@
         <v>2</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="13"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>20</v>
       </c>
@@ -1535,13 +1543,17 @@
         <v>3</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" s="13"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D12" s="13"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B15" s="11"/>
     </row>
   </sheetData>

</xml_diff>